<commit_message>
added db and tables and retrived some of the data from thrre
</commit_message>
<xml_diff>
--- a/webworkprogress_April_2019.xlsx
+++ b/webworkprogress_April_2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Probook4.DESKTOP-94EL945\Desktop\Azam soft Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\azam-st-laravell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +240,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -445,7 +451,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -531,6 +537,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -851,7 +872,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +991,8 @@
       <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="12"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="24"/>
       <c r="K6" s="20" t="s">
         <v>4</v>
@@ -1001,10 +1020,10 @@
       <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="12"/>
+      <c r="H7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="30"/>
       <c r="J7" s="24"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
@@ -1030,10 +1049,10 @@
       <c r="G8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="12"/>
+      <c r="H8" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="30"/>
       <c r="J8" s="24"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
@@ -1147,14 +1166,16 @@
       <c r="E13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
+      <c r="H13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="24"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -1174,14 +1195,16 @@
       <c r="E14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
+      <c r="H14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="12"/>
       <c r="J14" s="24"/>
       <c r="K14" s="21" t="s">
         <v>5</v>
@@ -1203,14 +1226,16 @@
       <c r="E15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
+      <c r="H15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12"/>
       <c r="J15" s="24"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -1221,12 +1246,8 @@
       <c r="B16" s="2">
         <v>11</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1624,7 +1645,7 @@
       <c r="M39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="K6:M13"/>
     <mergeCell ref="K14:M22"/>
@@ -1636,6 +1657,9 @@
     <mergeCell ref="B3:I4"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>